<commit_message>
improved random light selection, supported cube light
</commit_message>
<xml_diff>
--- a/perf.xlsx
+++ b/perf.xlsx
@@ -22,10 +22,10 @@
     <t>numBounces</t>
   </si>
   <si>
-    <t>photon tracing time (s)</t>
+    <t>render time (s)</t>
   </si>
   <si>
-    <t>render time (s)</t>
+    <t>photon tracing time (ms)</t>
   </si>
 </sst>
 </file>
@@ -370,14 +370,14 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="10.75" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.25" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -389,10 +389,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">

</xml_diff>